<commit_message>
Refactor fuzzy matching functions to use 'library' parameter
- Updated `process_match_value_and_lpu` and `process_budget_and_lpu` functions to replace the 'scorer' parameter with a 'library' parameter, allowing selection between "rapidfuzz" and "fuzzywuzzy".
- Adjusted calls to `fuzzy_match` within these functions to utilize the new 'library' parameter.
- Modified example scripts to reflect the changes in function signatures and demonstrate the use of the 'library' parameter.
</commit_message>
<xml_diff>
--- a/data/outputs/02_BASE_RESULTADO_VALIDADOR_LPU.xlsx
+++ b/data/outputs/02_BASE_RESULTADO_VALIDADOR_LPU.xlsx
@@ -627,14 +627,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>FORRO GESSO ACARTONADO</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>100</v>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -773,14 +767,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>FORRO GESSO ACARTONADO</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>100</v>
-      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -884,14 +872,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>FORRO GESSO ACARTONADO</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>100</v>
-      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -1065,14 +1047,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>100</v>
-      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -1316,14 +1292,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K24" t="n">
-        <v>100</v>
-      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -1392,14 +1362,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K26" t="n">
-        <v>100</v>
-      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -1678,14 +1642,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K34" t="n">
-        <v>100</v>
-      </c>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -1859,14 +1817,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K39" t="n">
-        <v>100</v>
-      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -1970,14 +1922,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K42" t="n">
-        <v>100</v>
-      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -3516,14 +3462,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K86" t="n">
-        <v>100</v>
-      </c>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
@@ -3837,14 +3777,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K95" t="n">
-        <v>100</v>
-      </c>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
@@ -3948,14 +3882,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K98" t="n">
-        <v>100</v>
-      </c>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
@@ -3989,14 +3917,8 @@
           <t>01</t>
         </is>
       </c>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>RETIRADA DE FORRO MANUAL</t>
-        </is>
-      </c>
-      <c r="K99" t="n">
-        <v>100</v>
-      </c>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>
@@ -5749,14 +5671,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J139" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K139" t="n">
-        <v>100</v>
-      </c>
+      <c r="J139" t="inlineStr"/>
+      <c r="K139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5845,7 +5761,7 @@
         </is>
       </c>
       <c r="K141" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="142">
@@ -6064,14 +5980,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J146" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K146" t="n">
-        <v>100</v>
-      </c>
+      <c r="J146" t="inlineStr"/>
+      <c r="K146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6784,14 +6694,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J162" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K162" t="n">
-        <v>100</v>
-      </c>
+      <c r="J162" t="inlineStr"/>
+      <c r="K162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6880,7 +6784,7 @@
         </is>
       </c>
       <c r="K164" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="165">
@@ -7150,7 +7054,7 @@
         </is>
       </c>
       <c r="K170" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="171">
@@ -7189,14 +7093,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J171" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K171" t="n">
-        <v>100</v>
-      </c>
+      <c r="J171" t="inlineStr"/>
+      <c r="K171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -7594,14 +7492,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J180" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K180" t="n">
-        <v>100</v>
-      </c>
+      <c r="J180" t="inlineStr"/>
+      <c r="K180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -8179,14 +8071,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J193" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K193" t="n">
-        <v>100</v>
-      </c>
+      <c r="J193" t="inlineStr"/>
+      <c r="K193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -8314,14 +8200,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J196" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K196" t="n">
-        <v>100</v>
-      </c>
+      <c r="J196" t="inlineStr"/>
+      <c r="K196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -9265,7 +9145,7 @@
         </is>
       </c>
       <c r="K217" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="218">
@@ -9529,14 +9409,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J223" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K223" t="n">
-        <v>100</v>
-      </c>
+      <c r="J223" t="inlineStr"/>
+      <c r="K223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -9760,7 +9634,7 @@
         </is>
       </c>
       <c r="K228" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="229">
@@ -9850,7 +9724,7 @@
         </is>
       </c>
       <c r="K230" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="231">
@@ -9934,14 +9808,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J232" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K232" t="n">
-        <v>100</v>
-      </c>
+      <c r="J232" t="inlineStr"/>
+      <c r="K232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -10030,7 +9898,7 @@
         </is>
       </c>
       <c r="K234" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="235">
@@ -10114,14 +9982,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J236" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K236" t="n">
-        <v>100</v>
-      </c>
+      <c r="J236" t="inlineStr"/>
+      <c r="K236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -10165,7 +10027,7 @@
         </is>
       </c>
       <c r="K237" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="238">
@@ -10525,7 +10387,7 @@
         </is>
       </c>
       <c r="K245" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="246">
@@ -11065,7 +10927,7 @@
         </is>
       </c>
       <c r="K257" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="258">
@@ -11509,14 +11371,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J267" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K267" t="n">
-        <v>100</v>
-      </c>
+      <c r="J267" t="inlineStr"/>
+      <c r="K267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -12325,7 +12181,7 @@
         </is>
       </c>
       <c r="K285" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="286">
@@ -12409,14 +12265,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J287" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K287" t="n">
-        <v>100</v>
-      </c>
+      <c r="J287" t="inlineStr"/>
+      <c r="K287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -12505,7 +12355,7 @@
         </is>
       </c>
       <c r="K289" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="290">
@@ -12640,7 +12490,7 @@
         </is>
       </c>
       <c r="K292" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="293">
@@ -13765,7 +13615,7 @@
         </is>
       </c>
       <c r="K317" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="318">
@@ -15160,7 +15010,7 @@
         </is>
       </c>
       <c r="K348" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="349">
@@ -15514,14 +15364,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J356" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K356" t="n">
-        <v>100</v>
-      </c>
+      <c r="J356" t="inlineStr"/>
+      <c r="K356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -15604,14 +15448,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J358" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K358" t="n">
-        <v>100</v>
-      </c>
+      <c r="J358" t="inlineStr"/>
+      <c r="K358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -15790,7 +15628,7 @@
         </is>
       </c>
       <c r="K362" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="363">
@@ -16549,14 +16387,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J379" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K379" t="n">
-        <v>100</v>
-      </c>
+      <c r="J379" t="inlineStr"/>
+      <c r="K379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -16600,7 +16432,7 @@
         </is>
       </c>
       <c r="K380" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="381">
@@ -16645,7 +16477,7 @@
         </is>
       </c>
       <c r="K381" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="382">
@@ -16864,14 +16696,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J386" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K386" t="n">
-        <v>100</v>
-      </c>
+      <c r="J386" t="inlineStr"/>
+      <c r="K386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -17449,14 +17275,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J399" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K399" t="n">
-        <v>100</v>
-      </c>
+      <c r="J399" t="inlineStr"/>
+      <c r="K399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -17545,7 +17365,7 @@
         </is>
       </c>
       <c r="K401" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="402">
@@ -17680,7 +17500,7 @@
         </is>
       </c>
       <c r="K404" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="405">
@@ -18985,7 +18805,7 @@
         </is>
       </c>
       <c r="K433" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="434">
@@ -19294,14 +19114,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J440" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K440" t="n">
-        <v>100</v>
-      </c>
+      <c r="J440" t="inlineStr"/>
+      <c r="K440" t="inlineStr"/>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
@@ -19480,7 +19294,7 @@
         </is>
       </c>
       <c r="K444" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="445">
@@ -19879,14 +19693,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J453" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K453" t="n">
-        <v>100</v>
-      </c>
+      <c r="J453" t="inlineStr"/>
+      <c r="K453" t="inlineStr"/>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
@@ -20155,7 +19963,7 @@
         </is>
       </c>
       <c r="K459" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="460">
@@ -20329,14 +20137,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J463" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K463" t="n">
-        <v>100</v>
-      </c>
+      <c r="J463" t="inlineStr"/>
+      <c r="K463" t="inlineStr"/>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
@@ -20374,14 +20176,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J464" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K464" t="n">
-        <v>100</v>
-      </c>
+      <c r="J464" t="inlineStr"/>
+      <c r="K464" t="inlineStr"/>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
@@ -20740,7 +20536,7 @@
         </is>
       </c>
       <c r="K472" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="473">
@@ -20785,7 +20581,7 @@
         </is>
       </c>
       <c r="K473" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="474">
@@ -20965,7 +20761,7 @@
         </is>
       </c>
       <c r="K477" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="478">
@@ -23164,14 +22960,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J526" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K526" t="n">
-        <v>100</v>
-      </c>
+      <c r="J526" t="inlineStr"/>
+      <c r="K526" t="inlineStr"/>
     </row>
     <row r="527">
       <c r="A527" t="inlineStr">
@@ -23260,7 +23050,7 @@
         </is>
       </c>
       <c r="K528" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="529">
@@ -23479,14 +23269,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J533" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K533" t="n">
-        <v>100</v>
-      </c>
+      <c r="J533" t="inlineStr"/>
+      <c r="K533" t="inlineStr"/>
     </row>
     <row r="534">
       <c r="A534" t="inlineStr">
@@ -24199,14 +23983,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J549" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K549" t="n">
-        <v>100</v>
-      </c>
+      <c r="J549" t="inlineStr"/>
+      <c r="K549" t="inlineStr"/>
     </row>
     <row r="550">
       <c r="A550" t="inlineStr">
@@ -24295,7 +24073,7 @@
         </is>
       </c>
       <c r="K551" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="552">
@@ -24565,7 +24343,7 @@
         </is>
       </c>
       <c r="K557" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="558">
@@ -24604,14 +24382,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J558" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K558" t="n">
-        <v>100</v>
-      </c>
+      <c r="J558" t="inlineStr"/>
+      <c r="K558" t="inlineStr"/>
     </row>
     <row r="559">
       <c r="A559" t="inlineStr">
@@ -25009,14 +24781,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J567" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K567" t="n">
-        <v>100</v>
-      </c>
+      <c r="J567" t="inlineStr"/>
+      <c r="K567" t="inlineStr"/>
     </row>
     <row r="568">
       <c r="A568" t="inlineStr">
@@ -25594,14 +25360,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J580" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K580" t="n">
-        <v>100</v>
-      </c>
+      <c r="J580" t="inlineStr"/>
+      <c r="K580" t="inlineStr"/>
     </row>
     <row r="581">
       <c r="A581" t="inlineStr">
@@ -25729,14 +25489,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J583" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K583" t="n">
-        <v>100</v>
-      </c>
+      <c r="J583" t="inlineStr"/>
+      <c r="K583" t="inlineStr"/>
     </row>
     <row r="584">
       <c r="A584" t="inlineStr">
@@ -26680,7 +26434,7 @@
         </is>
       </c>
       <c r="K604" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="605">
@@ -26944,14 +26698,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J610" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K610" t="n">
-        <v>100</v>
-      </c>
+      <c r="J610" t="inlineStr"/>
+      <c r="K610" t="inlineStr"/>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
@@ -27175,7 +26923,7 @@
         </is>
       </c>
       <c r="K615" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="616">
@@ -27265,7 +27013,7 @@
         </is>
       </c>
       <c r="K617" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="618">
@@ -27349,14 +27097,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J619" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K619" t="n">
-        <v>100</v>
-      </c>
+      <c r="J619" t="inlineStr"/>
+      <c r="K619" t="inlineStr"/>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
@@ -27445,7 +27187,7 @@
         </is>
       </c>
       <c r="K621" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="622">
@@ -27529,14 +27271,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J623" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K623" t="n">
-        <v>100</v>
-      </c>
+      <c r="J623" t="inlineStr"/>
+      <c r="K623" t="inlineStr"/>
     </row>
     <row r="624">
       <c r="A624" t="inlineStr">
@@ -27580,7 +27316,7 @@
         </is>
       </c>
       <c r="K624" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="625">
@@ -27940,7 +27676,7 @@
         </is>
       </c>
       <c r="K632" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="633">
@@ -28480,7 +28216,7 @@
         </is>
       </c>
       <c r="K644" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="645">
@@ -28924,14 +28660,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J654" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K654" t="n">
-        <v>100</v>
-      </c>
+      <c r="J654" t="inlineStr"/>
+      <c r="K654" t="inlineStr"/>
     </row>
     <row r="655">
       <c r="A655" t="inlineStr">
@@ -29740,7 +29470,7 @@
         </is>
       </c>
       <c r="K672" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="673">
@@ -29824,14 +29554,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J674" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K674" t="n">
-        <v>100</v>
-      </c>
+      <c r="J674" t="inlineStr"/>
+      <c r="K674" t="inlineStr"/>
     </row>
     <row r="675">
       <c r="A675" t="inlineStr">
@@ -29920,7 +29644,7 @@
         </is>
       </c>
       <c r="K676" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="677">
@@ -30055,7 +29779,7 @@
         </is>
       </c>
       <c r="K679" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="680">
@@ -31180,7 +30904,7 @@
         </is>
       </c>
       <c r="K704" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="705">
@@ -32575,7 +32299,7 @@
         </is>
       </c>
       <c r="K735" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="736">
@@ -32929,14 +32653,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J743" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K743" t="n">
-        <v>100</v>
-      </c>
+      <c r="J743" t="inlineStr"/>
+      <c r="K743" t="inlineStr"/>
     </row>
     <row r="744">
       <c r="A744" t="inlineStr">
@@ -33019,14 +32737,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J745" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K745" t="n">
-        <v>100</v>
-      </c>
+      <c r="J745" t="inlineStr"/>
+      <c r="K745" t="inlineStr"/>
     </row>
     <row r="746">
       <c r="A746" t="inlineStr">
@@ -33205,7 +32917,7 @@
         </is>
       </c>
       <c r="K749" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="750">
@@ -33964,14 +33676,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J766" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K766" t="n">
-        <v>100</v>
-      </c>
+      <c r="J766" t="inlineStr"/>
+      <c r="K766" t="inlineStr"/>
     </row>
     <row r="767">
       <c r="A767" t="inlineStr">
@@ -34015,7 +33721,7 @@
         </is>
       </c>
       <c r="K767" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="768">
@@ -34060,7 +33766,7 @@
         </is>
       </c>
       <c r="K768" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="769">
@@ -34279,14 +33985,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J773" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K773" t="n">
-        <v>100</v>
-      </c>
+      <c r="J773" t="inlineStr"/>
+      <c r="K773" t="inlineStr"/>
     </row>
     <row r="774">
       <c r="A774" t="inlineStr">
@@ -34864,14 +34564,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J786" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K786" t="n">
-        <v>100</v>
-      </c>
+      <c r="J786" t="inlineStr"/>
+      <c r="K786" t="inlineStr"/>
     </row>
     <row r="787">
       <c r="A787" t="inlineStr">
@@ -34960,7 +34654,7 @@
         </is>
       </c>
       <c r="K788" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="789">
@@ -35095,7 +34789,7 @@
         </is>
       </c>
       <c r="K791" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="792">
@@ -36400,7 +36094,7 @@
         </is>
       </c>
       <c r="K820" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="821">
@@ -36709,14 +36403,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J827" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K827" t="n">
-        <v>100</v>
-      </c>
+      <c r="J827" t="inlineStr"/>
+      <c r="K827" t="inlineStr"/>
     </row>
     <row r="828">
       <c r="A828" t="inlineStr">
@@ -36895,7 +36583,7 @@
         </is>
       </c>
       <c r="K831" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="832">
@@ -37294,14 +36982,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J840" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K840" t="n">
-        <v>100</v>
-      </c>
+      <c r="J840" t="inlineStr"/>
+      <c r="K840" t="inlineStr"/>
     </row>
     <row r="841">
       <c r="A841" t="inlineStr">
@@ -37570,7 +37252,7 @@
         </is>
       </c>
       <c r="K846" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="847">
@@ -37744,14 +37426,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J850" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K850" t="n">
-        <v>100</v>
-      </c>
+      <c r="J850" t="inlineStr"/>
+      <c r="K850" t="inlineStr"/>
     </row>
     <row r="851">
       <c r="A851" t="inlineStr">
@@ -37789,14 +37465,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J851" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K851" t="n">
-        <v>100</v>
-      </c>
+      <c r="J851" t="inlineStr"/>
+      <c r="K851" t="inlineStr"/>
     </row>
     <row r="852">
       <c r="A852" t="inlineStr">
@@ -38155,7 +37825,7 @@
         </is>
       </c>
       <c r="K859" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="860">
@@ -38200,7 +37870,7 @@
         </is>
       </c>
       <c r="K860" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="861">
@@ -38380,7 +38050,7 @@
         </is>
       </c>
       <c r="K864" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="865">
@@ -40579,14 +40249,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J913" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K913" t="n">
-        <v>100</v>
-      </c>
+      <c r="J913" t="inlineStr"/>
+      <c r="K913" t="inlineStr"/>
     </row>
     <row r="914">
       <c r="A914" t="inlineStr">
@@ -40675,7 +40339,7 @@
         </is>
       </c>
       <c r="K915" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="916">
@@ -40894,14 +40558,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J920" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K920" t="n">
-        <v>100</v>
-      </c>
+      <c r="J920" t="inlineStr"/>
+      <c r="K920" t="inlineStr"/>
     </row>
     <row r="921">
       <c r="A921" t="inlineStr">
@@ -41614,14 +41272,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J936" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K936" t="n">
-        <v>100</v>
-      </c>
+      <c r="J936" t="inlineStr"/>
+      <c r="K936" t="inlineStr"/>
     </row>
     <row r="937">
       <c r="A937" t="inlineStr">
@@ -41710,7 +41362,7 @@
         </is>
       </c>
       <c r="K938" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="939">
@@ -41980,7 +41632,7 @@
         </is>
       </c>
       <c r="K944" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="945">
@@ -42019,14 +41671,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J945" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K945" t="n">
-        <v>100</v>
-      </c>
+      <c r="J945" t="inlineStr"/>
+      <c r="K945" t="inlineStr"/>
     </row>
     <row r="946">
       <c r="A946" t="inlineStr">
@@ -42424,14 +42070,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J954" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K954" t="n">
-        <v>100</v>
-      </c>
+      <c r="J954" t="inlineStr"/>
+      <c r="K954" t="inlineStr"/>
     </row>
     <row r="955">
       <c r="A955" t="inlineStr">
@@ -43009,14 +42649,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J967" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K967" t="n">
-        <v>100</v>
-      </c>
+      <c r="J967" t="inlineStr"/>
+      <c r="K967" t="inlineStr"/>
     </row>
     <row r="968">
       <c r="A968" t="inlineStr">
@@ -43144,14 +42778,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J970" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K970" t="n">
-        <v>100</v>
-      </c>
+      <c r="J970" t="inlineStr"/>
+      <c r="K970" t="inlineStr"/>
     </row>
     <row r="971">
       <c r="A971" t="inlineStr">
@@ -44095,7 +43723,7 @@
         </is>
       </c>
       <c r="K991" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="992">
@@ -44359,14 +43987,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J997" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K997" t="n">
-        <v>100</v>
-      </c>
+      <c r="J997" t="inlineStr"/>
+      <c r="K997" t="inlineStr"/>
     </row>
     <row r="998">
       <c r="A998" t="inlineStr">
@@ -44590,7 +44212,7 @@
         </is>
       </c>
       <c r="K1002" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1003">
@@ -44680,7 +44302,7 @@
         </is>
       </c>
       <c r="K1004" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1005">
@@ -44764,14 +44386,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1006" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1006" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1006" t="inlineStr"/>
+      <c r="K1006" t="inlineStr"/>
     </row>
     <row r="1007">
       <c r="A1007" t="inlineStr">
@@ -44860,7 +44476,7 @@
         </is>
       </c>
       <c r="K1008" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1009">
@@ -44944,14 +44560,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1010" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1010" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1010" t="inlineStr"/>
+      <c r="K1010" t="inlineStr"/>
     </row>
     <row r="1011">
       <c r="A1011" t="inlineStr">
@@ -44995,7 +44605,7 @@
         </is>
       </c>
       <c r="K1011" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1012">
@@ -45355,7 +44965,7 @@
         </is>
       </c>
       <c r="K1019" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1020">
@@ -45895,7 +45505,7 @@
         </is>
       </c>
       <c r="K1031" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1032">
@@ -46339,14 +45949,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1041" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1041" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1041" t="inlineStr"/>
+      <c r="K1041" t="inlineStr"/>
     </row>
     <row r="1042">
       <c r="A1042" t="inlineStr">
@@ -47155,7 +46759,7 @@
         </is>
       </c>
       <c r="K1059" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1060">
@@ -47239,14 +46843,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1061" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1061" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1061" t="inlineStr"/>
+      <c r="K1061" t="inlineStr"/>
     </row>
     <row r="1062">
       <c r="A1062" t="inlineStr">
@@ -47335,7 +46933,7 @@
         </is>
       </c>
       <c r="K1063" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1064">
@@ -47470,7 +47068,7 @@
         </is>
       </c>
       <c r="K1066" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1067">
@@ -48595,7 +48193,7 @@
         </is>
       </c>
       <c r="K1091" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1092">
@@ -49990,7 +49588,7 @@
         </is>
       </c>
       <c r="K1122" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1123">
@@ -50344,14 +49942,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1130" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1130" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1130" t="inlineStr"/>
+      <c r="K1130" t="inlineStr"/>
     </row>
     <row r="1131">
       <c r="A1131" t="inlineStr">
@@ -50434,14 +50026,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1132" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1132" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1132" t="inlineStr"/>
+      <c r="K1132" t="inlineStr"/>
     </row>
     <row r="1133">
       <c r="A1133" t="inlineStr">
@@ -50620,7 +50206,7 @@
         </is>
       </c>
       <c r="K1136" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1137">
@@ -51379,14 +50965,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1153" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1153" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1153" t="inlineStr"/>
+      <c r="K1153" t="inlineStr"/>
     </row>
     <row r="1154">
       <c r="A1154" t="inlineStr">
@@ -51430,7 +51010,7 @@
         </is>
       </c>
       <c r="K1154" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1155">
@@ -51475,7 +51055,7 @@
         </is>
       </c>
       <c r="K1155" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1156">
@@ -51694,14 +51274,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1160" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1160" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1160" t="inlineStr"/>
+      <c r="K1160" t="inlineStr"/>
     </row>
     <row r="1161">
       <c r="A1161" t="inlineStr">
@@ -52279,14 +51853,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1173" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1173" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1173" t="inlineStr"/>
+      <c r="K1173" t="inlineStr"/>
     </row>
     <row r="1174">
       <c r="A1174" t="inlineStr">
@@ -52375,7 +51943,7 @@
         </is>
       </c>
       <c r="K1175" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1176">
@@ -52510,7 +52078,7 @@
         </is>
       </c>
       <c r="K1178" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1179">
@@ -53815,7 +53383,7 @@
         </is>
       </c>
       <c r="K1207" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1208">
@@ -54124,14 +53692,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1214" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1214" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1214" t="inlineStr"/>
+      <c r="K1214" t="inlineStr"/>
     </row>
     <row r="1215">
       <c r="A1215" t="inlineStr">
@@ -54310,7 +53872,7 @@
         </is>
       </c>
       <c r="K1218" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1219">
@@ -54709,14 +54271,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1227" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1227" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1227" t="inlineStr"/>
+      <c r="K1227" t="inlineStr"/>
     </row>
     <row r="1228">
       <c r="A1228" t="inlineStr">
@@ -54985,7 +54541,7 @@
         </is>
       </c>
       <c r="K1233" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1234">
@@ -55159,14 +54715,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1237" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1237" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1237" t="inlineStr"/>
+      <c r="K1237" t="inlineStr"/>
     </row>
     <row r="1238">
       <c r="A1238" t="inlineStr">
@@ -55204,14 +54754,8 @@
           <t>LPU</t>
         </is>
       </c>
-      <c r="J1238" t="inlineStr">
-        <is>
-          <t>REGULARIZACAO DE PISO COM REMOCAO</t>
-        </is>
-      </c>
-      <c r="K1238" t="n">
-        <v>100</v>
-      </c>
+      <c r="J1238" t="inlineStr"/>
+      <c r="K1238" t="inlineStr"/>
     </row>
     <row r="1239">
       <c r="A1239" t="inlineStr">
@@ -55570,7 +55114,7 @@
         </is>
       </c>
       <c r="K1246" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1247">
@@ -55615,7 +55159,7 @@
         </is>
       </c>
       <c r="K1247" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1248">
@@ -55795,7 +55339,7 @@
         </is>
       </c>
       <c r="K1251" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1252">

</xml_diff>